<commit_message>
added vehicle weight to vehicle master data
</commit_message>
<xml_diff>
--- a/template/Vehicle_Template.xlsx
+++ b/template/Vehicle_Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="11580"/>
+    <workbookView windowWidth="27945" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="bl_vendor" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Vehicle Number</t>
+  </si>
+  <si>
+    <t>Vehicle Weight</t>
   </si>
   <si>
     <t>Driver Name</t>
@@ -45,7 +48,7 @@
     <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="_-&quot;RM&quot;* #,##0_-;\-&quot;RM&quot;* #,##0_-;_-&quot;RM&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,13 +58,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -516,148 +512,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -983,36 +979,39 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85714285714286" defaultRowHeight="15" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="8.85714285714286" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.4285714285714" customWidth="1"/>
-    <col min="2" max="2" width="16.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="15.1428571428571" customWidth="1"/>
-    <col min="4" max="6" width="13.8571428571429" customWidth="1"/>
-    <col min="7" max="7" width="9.71428571428571" customWidth="1"/>
-    <col min="8" max="8" width="7" customWidth="1"/>
-    <col min="9" max="9" width="9.28571428571429" customWidth="1"/>
+    <col min="1" max="2" width="16.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="16.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="15.1428571428571" customWidth="1"/>
+    <col min="5" max="7" width="13.8571428571429" customWidth="1"/>
+    <col min="8" max="8" width="9.71428571428571" customWidth="1"/>
+    <col min="9" max="9" width="7" customWidth="1"/>
+    <col min="10" max="10" width="9.28571428571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>